<commit_message>
updated class act template
</commit_message>
<xml_diff>
--- a/templates/акт_на_классность.xlsx
+++ b/templates/акт_на_классность.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pronko\prj\Grader\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YUKI\3_Вирусы\Pronko_2\prj\Grader\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -151,22 +151,22 @@
     <t xml:space="preserve">Взвод: </t>
   </si>
   <si>
-    <t>полковник                    И.Полевщиков</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      На основании приказа командующего РВСН № 65 от 24 марта 2014 года в период с 21 по 25 апреля 2014 года
+    <t>Председатель комиссии:</t>
+  </si>
+  <si>
+    <t>подполковник</t>
+  </si>
+  <si>
+    <t>Федосеев А.Н.</t>
+  </si>
+  <si>
+    <t>полковник                            А. Казаков</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      На основании приказа командующего РВСН № 212 от 26 сентября 2014 года в период с 20 по 24 октября 2014 года
 руководствуясь «Инструкцией по проведению испытаний военнослужащих, проходящих военную службу в Вооруженных Силах Российской Федерации, для присвоения, изменения и лишения классной квалификации», произвели испытания военнослужащих – специалистов на присвоение (подтверждение, повышение) классной квалификации, проверили стаж практической работы и рассмотрели их служебные карточки.
      На основании результатов испытаний, данных о стаже практической работы по специальности, воинской дисциплины и служебных карточек комиссия
 определяет:</t>
-  </si>
-  <si>
-    <t>Председатель комиссии:</t>
-  </si>
-  <si>
-    <t>подполковник</t>
-  </si>
-  <si>
-    <t>Федосеев А.Н.</t>
   </si>
 </sst>
 </file>
@@ -710,7 +710,7 @@
   <dimension ref="A1:M68"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B10" sqref="B10:M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -746,7 +746,7 @@
     </row>
     <row r="3" spans="1:13" ht="20.25" x14ac:dyDescent="0.2">
       <c r="K3" s="17" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L3" s="17"/>
       <c r="M3" s="17"/>
@@ -844,7 +844,7 @@
     </row>
     <row r="10" spans="1:13" s="4" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="21" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
@@ -980,16 +980,16 @@
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>

</xml_diff>